<commit_message>
Different ways to fetch the HTML code of the email (Base64 image format)
</commit_message>
<xml_diff>
--- a/excel-reader-test.xlsx
+++ b/excel-reader-test.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajn/PycharmProjects/TaaraMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8D33D52-5AE9-9049-9424-6627360AA2C5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7736416-418E-1B49-837B-C2828339FBD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{BB956867-4E80-2549-9E3C-F98421C8FBD8}"/>
   </bookViews>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CE6897-0C0A-864B-B99E-A828F1F30F0D}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
+      <selection activeCell="H7" sqref="H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Final Push for any minute changes that might've crept in
</commit_message>
<xml_diff>
--- a/excel-reader-test.xlsx
+++ b/excel-reader-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10609"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajn/PycharmProjects/TaaraMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7736416-418E-1B49-837B-C2828339FBD5}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EC6A03-9DC4-4243-BCDC-59FA28F889C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{BB956867-4E80-2549-9E3C-F98421C8FBD8}"/>
   </bookViews>
@@ -550,7 +550,7 @@
   <dimension ref="A1:P5"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="H7" sqref="H7"/>
+      <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
Added the custom name feature
</commit_message>
<xml_diff>
--- a/excel-reader-test.xlsx
+++ b/excel-reader-test.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10715"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10812"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/rajn/PycharmProjects/TaaraMail/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12EC6A03-9DC4-4243-BCDC-59FA28F889C3}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{67FEDA52-F99E-834A-9166-D2BD97EF3F75}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="3180" yWindow="2060" windowWidth="27640" windowHeight="16940" xr2:uid="{BB956867-4E80-2549-9E3C-F98421C8FBD8}"/>
   </bookViews>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D1CE6897-0C0A-864B-B99E-A828F1F30F0D}">
   <dimension ref="A1:P5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" zoomScale="267" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>